<commit_message>
Version estable para master
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\py-ersonal_email\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B3EDC2-F7CD-408D-B008-7B51FE0CE2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF36C99-6208-4C7B-B7F6-DFD05B8EF78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>From</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>plain</t>
+  </si>
+  <si>
+    <t>Password is</t>
+  </si>
+  <si>
+    <t>encrypted</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -193,11 +202,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,9 +238,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -236,6 +251,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -661,15 +685,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="50.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="137.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="50.7109375" style="1"/>
   </cols>
@@ -681,98 +705,112 @@
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="3" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="B3" s="14"/>
+    </row>
+    <row r="4" spans="1:2" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+    <row r="6" spans="1:2" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:2" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="10" spans="1:2" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:XFD1">
+  <conditionalFormatting sqref="B1:XFD2">
     <cfRule type="expression" dxfId="7" priority="8">
       <formula>B1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:XFD2">
+  <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="expression" dxfId="6" priority="7">
-      <formula>B2&lt;&gt;""</formula>
+      <formula>B3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:XFD4">
+  <conditionalFormatting sqref="C5:XFD5">
     <cfRule type="expression" dxfId="5" priority="6">
-      <formula>C4&lt;&gt;""</formula>
+      <formula>C5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:XFD5">
+  <conditionalFormatting sqref="B6:XFD6">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>B5&lt;&gt;""</formula>
+      <formula>B6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:XFD7">
+  <conditionalFormatting sqref="B8:XFD8">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>B7&lt;&gt;""</formula>
+      <formula>B8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:XFD9">
+  <conditionalFormatting sqref="B10:XFD10">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>B9&lt;&gt;""</formula>
+      <formula>B10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:XFD11">
+  <conditionalFormatting sqref="B12:XFD12">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>B11&lt;&gt;""</formula>
+      <formula>B12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
+  <conditionalFormatting sqref="B5">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>B4&lt;&gt;""</formula>
+      <formula>B5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEACD274-F06F-44DF-AC48-52CBCA0476F1}">
           <x14:formula1>
             <xm:f>list_data!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
+          <xm:sqref>B11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{37B27788-CF1D-4264-9F84-017AE437959E}">
+          <x14:formula1>
+            <xm:f>list_data!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -782,30 +820,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8D02CE-9025-439A-BF0B-6C4B3BA40769}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correccion de archivo readme.md
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\py-ersonal_email\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF36C99-6208-4C7B-B7F6-DFD05B8EF78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D01E0B4-6072-40F8-8038-9AB6B0B38082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -688,7 +688,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="50.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>